<commit_message>
Add Kss to parameter files for simulation.  Clean up formatting and naming in parameter files
</commit_message>
<xml_diff>
--- a/parameters/ModelG_Atezolizumab_Params.xlsx
+++ b/parameters/ModelG_Atezolizumab_Params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\TMDD_EndogenousLigand\parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/git/TMDD_EndogenousLigand/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8E0D26-AF33-4DF9-AA71-77F146E21209}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC017F8-2D24-C543-A936-6909547DF516}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="CL_">Sheet1!$F$4</definedName>
     <definedName name="Dose">Sheet1!#REF!</definedName>
     <definedName name="eps">Sheet1!#REF!</definedName>
-    <definedName name="Imax">Sheet1!$F$20</definedName>
+    <definedName name="Imax">Sheet1!#REF!</definedName>
     <definedName name="k12D">Sheet1!#REF!</definedName>
     <definedName name="k13D">Sheet1!#REF!</definedName>
     <definedName name="k13d_prop">Sheet1!#REF!</definedName>
@@ -38,7 +38,7 @@
     <definedName name="k31D_thurber">Sheet1!#REF!</definedName>
     <definedName name="k31M">Sheet1!#REF!</definedName>
     <definedName name="Kd">Sheet1!#REF!</definedName>
-    <definedName name="Kd_DT">Sheet1!$F$23</definedName>
+    <definedName name="Kd_DT">Sheet1!$F$22</definedName>
     <definedName name="Kd_TL">Sheet1!$F$30</definedName>
     <definedName name="kd_ugml">Sheet1!#REF!</definedName>
     <definedName name="keD">Sheet1!#REF!</definedName>
@@ -46,7 +46,7 @@
     <definedName name="keDM3">Sheet1!#REF!</definedName>
     <definedName name="keDMtot">Sheet1!#REF!</definedName>
     <definedName name="keDS1">Sheet1!#REF!</definedName>
-    <definedName name="keDT">Sheet1!$F$21</definedName>
+    <definedName name="keDT">Sheet1!$F$20</definedName>
     <definedName name="keL">Sheet1!$F$27</definedName>
     <definedName name="keM">Sheet1!#REF!</definedName>
     <definedName name="keM3_">Sheet1!#REF!</definedName>
@@ -55,8 +55,10 @@
     <definedName name="Km">Sheet1!$F$12</definedName>
     <definedName name="koff">Sheet1!#REF!</definedName>
     <definedName name="koff_DT">Sheet1!$F$24</definedName>
-    <definedName name="koff_TL">Sheet1!$F$31</definedName>
+    <definedName name="koff_TL">Sheet1!$F$32</definedName>
     <definedName name="kon">Sheet1!#REF!</definedName>
+    <definedName name="kon_DT">Sheet1!$E$25</definedName>
+    <definedName name="kon_DTn">Sheet1!$F$25</definedName>
     <definedName name="kshed">Sheet1!#REF!</definedName>
     <definedName name="kshedDM1">Sheet1!#REF!</definedName>
     <definedName name="kshedDM3">Sheet1!#REF!</definedName>
@@ -67,7 +69,7 @@
     <definedName name="ksynTs">Sheet1!$F$18</definedName>
     <definedName name="ksynTs_ngml">Sheet1!#REF!</definedName>
     <definedName name="L0">Sheet1!$F$29</definedName>
-    <definedName name="m">Sheet1!$F$33</definedName>
+    <definedName name="m">Sheet1!$F$34</definedName>
     <definedName name="M10_">Sheet1!#REF!</definedName>
     <definedName name="M30_">Sheet1!#REF!</definedName>
     <definedName name="Mfrac">Sheet1!#REF!</definedName>
@@ -105,7 +107,7 @@
     <definedName name="VtumDS">Sheet1!#REF!</definedName>
     <definedName name="VtumS">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -124,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="95">
   <si>
     <t>Parameter</t>
   </si>
@@ -255,9 +257,6 @@
     <t>keT</t>
   </si>
   <si>
-    <t>Imax</t>
-  </si>
-  <si>
     <t>ug/(ml*d)</t>
   </si>
   <si>
@@ -276,9 +275,6 @@
     <t>Elimination Rate</t>
   </si>
   <si>
-    <t>Gibiansky12 - Table 2 doi 10.1007/s10928-011-9227-z</t>
-  </si>
-  <si>
     <t>Synthesis Rate</t>
   </si>
   <si>
@@ -306,9 +302,6 @@
     <t>Turnover</t>
   </si>
   <si>
-    <t>"Inhibition"</t>
-  </si>
-  <si>
     <t>MWT</t>
   </si>
   <si>
@@ -406,6 +399,18 @@
   </si>
   <si>
     <t>From Pembrolizumab model</t>
+  </si>
+  <si>
+    <t>Kss_DT</t>
+  </si>
+  <si>
+    <t>Equilibration Constant</t>
+  </si>
+  <si>
+    <t>Kss_TL</t>
+  </si>
+  <si>
+    <t>Nonlinear Elim Vmax</t>
   </si>
 </sst>
 </file>
@@ -416,13 +421,20 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -445,13 +457,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -459,6 +464,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -510,32 +516,32 @@
   </borders>
   <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -567,31 +573,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -606,7 +612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -618,29 +624,20 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="25">
@@ -1182,8 +1179,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J32" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J33" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ParamType" dataDxfId="8"/>
@@ -1524,28 +1521,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="20" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="21" customWidth="1"/>
-    <col min="7" max="7" width="9.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="21" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="2" customWidth="1"/>
     <col min="9" max="9" width="25.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="50.375" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="10.875" style="4"/>
+    <col min="10" max="10" width="50.33203125" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -1577,7 +1574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1588,10 +1585,10 @@
         <v>26</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -1600,17 +1597,17 @@
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I2" s="20" t="str">
         <f t="shared" ref="I2:I3" ca="1" si="0">_xlfn.IFNA(_xlfn.FORMULATEXT(F2),"")</f>
         <v/>
       </c>
       <c r="J2" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1621,10 +1618,10 @@
         <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -1633,17 +1630,17 @@
         <v>4</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I3" s="20" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="J3" s="34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="25" customFormat="1">
+      <c r="J3" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1669,14 +1666,14 @@
         <v>17</v>
       </c>
       <c r="I4" s="13" t="str">
-        <f t="shared" ref="I4:I23" ca="1" si="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F4),"")</f>
+        <f t="shared" ref="I4:I22" ca="1" si="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F4),"")</f>
         <v/>
       </c>
-      <c r="J4" s="34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="25" customFormat="1">
+      <c r="J4" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1705,11 +1702,11 @@
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="J5" s="34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="25" customFormat="1">
+      <c r="J5" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1725,7 +1722,7 @@
       <c r="E6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="21">
         <v>0.54600000000000004</v>
       </c>
       <c r="G6" s="23" t="s">
@@ -1738,11 +1735,11 @@
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="J6" s="34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="25" customFormat="1">
+      <c r="J6" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1771,11 +1768,11 @@
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="J7" s="34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="25" customFormat="1">
+      <c r="J7" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1786,7 +1783,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>37</v>
@@ -1807,7 +1804,7 @@
       </c>
       <c r="J8" s="24"/>
     </row>
-    <row r="9" spans="1:10" s="25" customFormat="1">
+    <row r="9" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1821,13 +1818,15 @@
         <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="22">
         <f>Q_/V1_</f>
         <v>0.16646341463414635</v>
       </c>
-      <c r="G9" s="23"/>
+      <c r="G9" s="23" t="s">
+        <v>4</v>
+      </c>
       <c r="H9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1837,7 +1836,7 @@
       </c>
       <c r="J9" s="24"/>
     </row>
-    <row r="10" spans="1:10" s="25" customFormat="1">
+    <row r="10" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1851,13 +1850,15 @@
         <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="22">
         <f>Q_/V2_</f>
         <v>0.15041322314049588</v>
       </c>
-      <c r="G10" s="23"/>
+      <c r="G10" s="23" t="s">
+        <v>4</v>
+      </c>
       <c r="H10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1867,7 +1868,7 @@
       </c>
       <c r="J10" s="24"/>
     </row>
-    <row r="11" spans="1:10" s="25" customFormat="1">
+    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1878,16 +1879,16 @@
         <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F11" s="26">
         <v>0</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>17</v>
@@ -1897,10 +1898,10 @@
         <v/>
       </c>
       <c r="J11" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="25" customFormat="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1911,16 +1912,16 @@
         <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F12" s="26">
         <v>1</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>17</v>
@@ -1930,10 +1931,10 @@
         <v/>
       </c>
       <c r="J12" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="25" customFormat="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1944,7 +1945,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>40</v>
@@ -1965,7 +1966,7 @@
       </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" s="25" customFormat="1">
+    <row r="14" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1976,7 +1977,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>41</v>
@@ -1996,7 +1997,7 @@
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" s="25" customFormat="1">
+    <row r="15" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2029,21 +2030,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="25" customFormat="1">
+    <row r="16" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>84</v>
+      <c r="C16" s="28" t="s">
+        <v>81</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F16" s="26">
         <v>33</v>
@@ -2059,10 +2060,10 @@
         <v/>
       </c>
       <c r="J16" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="25" customFormat="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2070,13 +2071,13 @@
         <v>36</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F17" s="26">
         <v>32</v>
@@ -2095,21 +2096,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="25" customFormat="1">
+    <row r="18" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>86</v>
+        <v>57</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F18" s="27">
         <v>0.45</v>
@@ -2118,27 +2119,27 @@
         <v>7</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I18" s="35" t="s">
-        <v>90</v>
+        <v>86</v>
+      </c>
+      <c r="I18" s="30" t="s">
+        <v>87</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="25" customFormat="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>86</v>
+        <v>57</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>42</v>
@@ -2157,156 +2158,155 @@
         <v/>
       </c>
       <c r="J19" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="25" customFormat="1">
-      <c r="A20" s="30">
-        <v>20</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="32">
-        <v>0.93899999999999995</v>
-      </c>
-      <c r="G20" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" s="30" t="s">
-        <v>17</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="22">
+        <v>6</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="I20" s="13" t="str">
         <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F20),"")</f>
         <v/>
       </c>
       <c r="J20" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="25" customFormat="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>86</v>
+        <v>57</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="22">
-        <v>6</v>
+        <v>62</v>
+      </c>
+      <c r="F21" s="21">
+        <v>7.47</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I21" s="13" t="str">
         <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F21),"")</f>
         <v/>
       </c>
       <c r="J21" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="25" customFormat="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>86</v>
+        <v>36</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="28">
-        <v>7.47</v>
+        <v>50</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.4</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>15</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I22" s="13" t="str">
-        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F22),"")</f>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="J22" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="25" customFormat="1">
+      <c r="J22" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>24</v>
+        <v>24.5</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>86</v>
+      <c r="C23" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="8">
-        <v>0.4</v>
+        <v>91</v>
+      </c>
+      <c r="F23" s="2">
+        <f>(koff_DT+keDT)/kon_DTn</f>
+        <v>1.2</v>
       </c>
       <c r="G23" s="23" t="s">
         <v>15</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I23" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="25" customFormat="1">
+        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F23),"")</f>
+        <v>=(koff_DT+keDT)/kon_DTn</v>
+      </c>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="29" t="s">
-        <v>86</v>
+      <c r="C24" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F24" s="15">
         <v>3</v>
@@ -2323,21 +2323,21 @@
       </c>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" s="25" customFormat="1">
+    <row r="25" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="29" t="s">
-        <v>86</v>
+      <c r="C25" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="F25" s="17">
         <f>koff_DT/Kd_DT</f>
@@ -2355,21 +2355,21 @@
       </c>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" s="25" customFormat="1">
+    <row r="26" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>27</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F26" s="16">
         <v>0.03</v>
@@ -2382,24 +2382,24 @@
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="25" customFormat="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>28</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F27" s="15">
         <v>3</v>
@@ -2411,28 +2411,28 @@
         <v>18</v>
       </c>
       <c r="I27" s="13" t="str">
-        <f t="shared" ref="I27:I32" ca="1" si="3">_xlfn.IFNA(_xlfn.FORMULATEXT(F27),"")</f>
+        <f t="shared" ref="I27:I33" ca="1" si="3">_xlfn.IFNA(_xlfn.FORMULATEXT(F27),"")</f>
         <v/>
       </c>
       <c r="J27" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="25" customFormat="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>29</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F28" s="21">
         <v>0</v>
@@ -2445,24 +2445,24 @@
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="25" customFormat="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>30</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>35</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F29" s="15">
         <v>9.9000000000000008E-3</v>
@@ -2471,14 +2471,14 @@
         <v>15</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>31</v>
       </c>
@@ -2486,13 +2486,13 @@
         <v>36</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F30" s="15">
         <v>10</v>
@@ -2509,79 +2509,111 @@
       </c>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
+        <v>31.5</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="15">
+        <f>(koff_TL+F28)/F33</f>
+        <v>10</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I31" s="13" t="str">
+        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F31),"")</f>
+        <v>=(koff_TL+F28)/F33</v>
+      </c>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
         <v>32</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="18">
-        <v>5</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="19" t="str">
-        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F31),"")</f>
-        <v/>
-      </c>
-      <c r="J31" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="6">
-        <v>33</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F32" s="15">
+        <v>67</v>
+      </c>
+      <c r="F32" s="18">
+        <v>5</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="19" t="str">
+        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F32),"")</f>
+        <v/>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>33</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="15">
         <f>koff_TL/Kd_TL</f>
         <v>0.5</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G33" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="13" t="str">
+      <c r="I33" s="13" t="str">
         <f t="shared" ca="1" si="3"/>
         <v>=koff_TL/Kd_TL</v>
       </c>
-      <c r="J32" s="14"/>
+      <c r="J33" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="F214">
+  <conditionalFormatting sqref="F215">
     <cfRule type="containsText" dxfId="34" priority="54" operator="containsText" text="derived">
-      <formula>NOT(ISERROR(SEARCH("derived",F214)))</formula>
+      <formula>NOT(ISERROR(SEARCH("derived",F215)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:K1 A33:K1048576 E13:K14 B8:K12 G22:K22 A4:A32 B22:E23 G23:I23 K23 B4:I7 K2:K7 B15:K21 B24:K32">
+  <conditionalFormatting sqref="A1:K1 A34:K1048576 E13:K14 B8:K12 G21:K21 B21:E23 K22:K23 B4:I7 K2:K7 G22:I23 B24:K33 A4:A33 B15:K20">
     <cfRule type="containsText" dxfId="33" priority="51" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",A1)))</formula>
     </cfRule>
@@ -2656,14 +2688,14 @@
       <formula>NOT(ISERROR(SEARCH("calc",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23">
+  <conditionalFormatting sqref="F22:F23">
     <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="calc">
-      <formula>NOT(ISERROR(SEARCH("calc",F23)))</formula>
+      <formula>NOT(ISERROR(SEARCH("calc",F22)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J23">
+  <conditionalFormatting sqref="J22:J23">
     <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="calc">
-      <formula>NOT(ISERROR(SEARCH("calc",J23)))</formula>
+      <formula>NOT(ISERROR(SEARCH("calc",J22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">

</xml_diff>

<commit_message>
good agreement for mem and sol + explain how Lfold increase relates to SCIM
</commit_message>
<xml_diff>
--- a/parameters/ModelG_Atezolizumab_Params.xlsx
+++ b/parameters/ModelG_Atezolizumab_Params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/git/TMDD_EndogenousLigand/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC017F8-2D24-C543-A936-6909547DF516}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2CC99E-0295-1C49-9053-0C82CE8E6A02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1524,7 +1524,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2435,7 +2435,8 @@
         <v>64</v>
       </c>
       <c r="F28" s="21">
-        <v>0</v>
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>4</v>
@@ -2527,7 +2528,7 @@
       </c>
       <c r="F31" s="15">
         <f>(koff_TL+F28)/F33</f>
-        <v>10</v>
+        <v>10.066666666666666</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
creating first draft of figures for manuscript
</commit_message>
<xml_diff>
--- a/parameters/ModelG_Atezolizumab_Params.xlsx
+++ b/parameters/ModelG_Atezolizumab_Params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/git/TMDD_EndogenousLigand/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4668068-F6F6-5F4C-99C7-D917222D489E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE766E5D-37E7-E342-B1FE-4AFDD6D651AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1523,7 +1523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="99" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixing Pembro and Atezo params
</commit_message>
<xml_diff>
--- a/parameters/ModelG_Atezolizumab_Params.xlsx
+++ b/parameters/ModelG_Atezolizumab_Params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/git/TMDD_EndogenousLigand/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9653A7-0B5A-BA48-B840-556682C645A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E79B01C-7427-414D-B076-6B2157965672}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="2440" windowWidth="28800" windowHeight="14920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,13 @@
     <definedName name="ABCdrug">Sheet1!#REF!</definedName>
     <definedName name="ABCsol">Sheet1!#REF!</definedName>
     <definedName name="Cavg">Sheet1!#REF!</definedName>
-    <definedName name="CL">Sheet1!#REF!</definedName>
+    <definedName name="CL">Sheet1!$F$4</definedName>
     <definedName name="CL_">Sheet1!$F$4</definedName>
     <definedName name="Dose">Sheet1!#REF!</definedName>
     <definedName name="eps">Sheet1!#REF!</definedName>
+    <definedName name="F">Sheet1!$F$2</definedName>
     <definedName name="Imax">Sheet1!#REF!</definedName>
+    <definedName name="k12_">Sheet1!$F$9</definedName>
     <definedName name="k12D">Sheet1!#REF!</definedName>
     <definedName name="k13D">Sheet1!#REF!</definedName>
     <definedName name="k13d_prop">Sheet1!#REF!</definedName>
@@ -32,56 +34,66 @@
     <definedName name="k13DS">Sheet1!#REF!</definedName>
     <definedName name="k13M">Sheet1!#REF!</definedName>
     <definedName name="k13S">Sheet1!#REF!</definedName>
+    <definedName name="k21_">Sheet1!$F$10</definedName>
     <definedName name="k21D">Sheet1!#REF!</definedName>
     <definedName name="k31D">Sheet1!#REF!</definedName>
     <definedName name="k31D_prop">Sheet1!#REF!</definedName>
     <definedName name="k31D_thurber">Sheet1!#REF!</definedName>
     <definedName name="k31M">Sheet1!#REF!</definedName>
+    <definedName name="ka">Sheet1!$F$3</definedName>
     <definedName name="Kd">Sheet1!#REF!</definedName>
-    <definedName name="Kd_DT">Sheet1!$F$22</definedName>
-    <definedName name="Kd_TL">Sheet1!$F$30</definedName>
+    <definedName name="Kd_DT">Sheet1!$F$24</definedName>
+    <definedName name="Kd_TL">Sheet1!$F$31</definedName>
     <definedName name="kd_ugml">Sheet1!#REF!</definedName>
-    <definedName name="keD">Sheet1!#REF!</definedName>
+    <definedName name="keD">Sheet1!$F$8</definedName>
     <definedName name="keD3_">Sheet1!#REF!</definedName>
     <definedName name="keDM3">Sheet1!#REF!</definedName>
     <definedName name="keDMtot">Sheet1!#REF!</definedName>
     <definedName name="keDS1">Sheet1!#REF!</definedName>
     <definedName name="keDT">Sheet1!$F$20</definedName>
-    <definedName name="keL">Sheet1!$F$27</definedName>
+    <definedName name="keL">Sheet1!$F$29</definedName>
     <definedName name="keM">Sheet1!#REF!</definedName>
     <definedName name="keM3_">Sheet1!#REF!</definedName>
     <definedName name="keT">Sheet1!$F$19</definedName>
+    <definedName name="keTL">Sheet1!$F$30</definedName>
     <definedName name="keTs">Sheet1!$F$19</definedName>
-    <definedName name="Km">Sheet1!$F$12</definedName>
+    <definedName name="Km">Sheet1!$F$14</definedName>
+    <definedName name="Km_ugml">Sheet1!$F$12</definedName>
     <definedName name="koff">Sheet1!#REF!</definedName>
-    <definedName name="koff_DT">Sheet1!$F$24</definedName>
-    <definedName name="koff_TL">Sheet1!$F$32</definedName>
+    <definedName name="koff_DT">Sheet1!$F$26</definedName>
+    <definedName name="koff_TL">Sheet1!$F$33</definedName>
     <definedName name="kon">Sheet1!#REF!</definedName>
-    <definedName name="kon_DT">Sheet1!$E$25</definedName>
-    <definedName name="kon_DTn">Sheet1!$F$25</definedName>
+    <definedName name="kon_DT">Sheet1!$F$27</definedName>
+    <definedName name="kon_DTn">Sheet1!$F$27</definedName>
+    <definedName name="kon_TL">Sheet1!$F$34</definedName>
     <definedName name="kshed">Sheet1!#REF!</definedName>
     <definedName name="kshedDM1">Sheet1!#REF!</definedName>
     <definedName name="kshedDM3">Sheet1!#REF!</definedName>
     <definedName name="kshedM1">Sheet1!#REF!</definedName>
     <definedName name="kshedM3">Sheet1!#REF!</definedName>
+    <definedName name="Kss_DT">Sheet1!$F$25</definedName>
+    <definedName name="Kss_TL">Sheet1!$F$32</definedName>
     <definedName name="ksyn_ngml">Sheet1!#REF!</definedName>
-    <definedName name="ksynL">Sheet1!$F$26</definedName>
+    <definedName name="ksynL">Sheet1!$F$28</definedName>
+    <definedName name="ksynT">Sheet1!$F$18</definedName>
     <definedName name="ksynTs">Sheet1!$F$18</definedName>
     <definedName name="ksynTs_ngml">Sheet1!#REF!</definedName>
-    <definedName name="L0">Sheet1!$F$29</definedName>
-    <definedName name="m">Sheet1!$F$34</definedName>
+    <definedName name="L0">Sheet1!$F$22</definedName>
+    <definedName name="m">Sheet1!$F$35</definedName>
     <definedName name="M10_">Sheet1!#REF!</definedName>
     <definedName name="M30_">Sheet1!#REF!</definedName>
     <definedName name="Mfrac">Sheet1!#REF!</definedName>
     <definedName name="MWD">Sheet1!$F$15</definedName>
+    <definedName name="MWL">Sheet1!$F$17</definedName>
     <definedName name="MWLm">Sheet1!#REF!</definedName>
     <definedName name="MWLs">Sheet1!$F$17</definedName>
     <definedName name="MWS">Sheet1!#REF!</definedName>
+    <definedName name="MWT">Sheet1!$F$16</definedName>
     <definedName name="MWTm">Sheet1!#REF!</definedName>
     <definedName name="MWTs">Sheet1!$F$16</definedName>
     <definedName name="Npercell">Sheet1!#REF!</definedName>
     <definedName name="P">Sheet1!#REF!</definedName>
-    <definedName name="Q">Sheet1!#REF!</definedName>
+    <definedName name="Q">Sheet1!$F$6</definedName>
     <definedName name="Q_">Sheet1!$F$6</definedName>
     <definedName name="Rcap">Sheet1!#REF!</definedName>
     <definedName name="Rho">Sheet1!#REF!</definedName>
@@ -89,8 +101,10 @@
     <definedName name="Rkrogh">Sheet1!#REF!</definedName>
     <definedName name="S10_">Sheet1!#REF!</definedName>
     <definedName name="S1acc">Sheet1!#REF!</definedName>
+    <definedName name="T0">Sheet1!$F$21</definedName>
     <definedName name="Tau">Sheet1!#REF!</definedName>
     <definedName name="Tfrac">Sheet1!#REF!</definedName>
+    <definedName name="TL0">Sheet1!$F$23</definedName>
     <definedName name="V1_">Sheet1!$F$5</definedName>
     <definedName name="V2_">Sheet1!$F$7</definedName>
     <definedName name="Vc">Sheet1!#REF!</definedName>
@@ -100,7 +114,8 @@
     <definedName name="VD2_">Sheet1!#REF!</definedName>
     <definedName name="VD3_">Sheet1!#REF!</definedName>
     <definedName name="VDS1_">Sheet1!#REF!</definedName>
-    <definedName name="Vm">Sheet1!$F$11</definedName>
+    <definedName name="Vm">Sheet1!$F$13</definedName>
+    <definedName name="Vm_ugml">Sheet1!$F$11</definedName>
     <definedName name="Vp">Sheet1!#REF!</definedName>
     <definedName name="VS1_">Sheet1!#REF!</definedName>
     <definedName name="Vtum">Sheet1!#REF!</definedName>
@@ -126,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="100">
   <si>
     <t>Parameter</t>
   </si>
@@ -269,9 +284,6 @@
     <t>k21</t>
   </si>
   <si>
-    <t>Gibiansky12 - Table 1 doi 10.1007/s10928-011-9227-z</t>
-  </si>
-  <si>
     <t>Elimination Rate</t>
   </si>
   <si>
@@ -359,18 +371,12 @@
     <t>Km_ugml</t>
   </si>
   <si>
-    <t>linear PK</t>
-  </si>
-  <si>
     <t>linear Elim Vmax</t>
   </si>
   <si>
     <t>google search (runs at higher mol weight on SDS PAGE due to post-translational modifications</t>
   </si>
   <si>
-    <t>from Atezolizumab model</t>
-  </si>
-  <si>
     <t>Target (PD-L1)</t>
   </si>
   <si>
@@ -389,15 +395,6 @@
     <t>calculated</t>
   </si>
   <si>
-    <t>Baseline level*kshed</t>
-  </si>
-  <si>
-    <t>from  Pembro_G_model</t>
-  </si>
-  <si>
-    <t>From Pembrolizumab model</t>
-  </si>
-  <si>
     <t>Kss_DT</t>
   </si>
   <si>
@@ -411,23 +408,62 @@
   </si>
   <si>
     <t>Stroh17 - 10.1002/cpt.587</t>
+  </si>
+  <si>
+    <t>from Atezolizumab model in Ahmed19 in circulation - https://doi.org/10.1007/s10928-019-09638-3</t>
+  </si>
+  <si>
+    <t>TL0</t>
+  </si>
+  <si>
+    <t>Complex</t>
+  </si>
+  <si>
+    <t>Compelx</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>from Pembrolizumab model in Ahmed19 in circulation - https://doi.org/10.1007/s10928-019-09638-3</t>
+  </si>
+  <si>
+    <t>typical value</t>
+  </si>
+  <si>
+    <t>set to 1 not used</t>
+  </si>
+  <si>
+    <t>Lindauer17 - 10.1002/psp4.12130 - .144/h * 24h/d</t>
+  </si>
+  <si>
+    <t>From target calculation (keT) from ModelG_Tocilizumab file</t>
+  </si>
+  <si>
+    <t>From target calculation (keTL) from ModelG_Tocilizumab file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000000"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -473,25 +509,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -516,32 +546,32 @@
   </borders>
   <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -567,38 +597,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -612,7 +621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -624,20 +633,23 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="25">
@@ -670,6 +682,237 @@
   <dxfs count="35">
     <dxf>
       <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -927,237 +1170,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF800000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1179,21 +1191,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J33" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J34" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="A1:J34" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ParamType" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Molecule" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Value" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Units" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Source" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Formula" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ParamType" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Molecule" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Value" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Units" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Source" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Formula" dataDxfId="24">
       <calculatedColumnFormula>_xlfn.IFNA(_xlfn.FORMULATEXT(F2),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comment or Reference" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comment or Reference" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1521,10 +1533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="99" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1534,7 +1546,7 @@
     <col min="3" max="3" width="20" style="3" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="14" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="2" customWidth="1"/>
     <col min="9" max="9" width="25.5" style="2" customWidth="1"/>
@@ -1558,7 +1570,7 @@
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -1585,10 +1597,10 @@
         <v>26</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -1597,9 +1609,9 @@
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="20" t="str">
+        <v>72</v>
+      </c>
+      <c r="I2" s="13" t="str">
         <f t="shared" ref="I2:I3" ca="1" si="0">_xlfn.IFNA(_xlfn.FORMULATEXT(F2),"")</f>
         <v/>
       </c>
@@ -1616,10 +1628,10 @@
         <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -1628,15 +1640,15 @@
         <v>4</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="20" t="str">
+        <v>72</v>
+      </c>
+      <c r="I3" s="13" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="J3" s="29"/>
-    </row>
-    <row r="4" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1649,27 +1661,27 @@
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="19">
         <v>0.2</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="16" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="13" t="str">
-        <f t="shared" ref="I4:I22" ca="1" si="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F4),"")</f>
+      <c r="I4" s="11" t="str">
+        <f t="shared" ref="I4:I24" ca="1" si="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F4),"")</f>
         <v/>
       </c>
-      <c r="J4" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1682,27 +1694,27 @@
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="19">
         <v>3.28</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="13" t="str">
+      <c r="I5" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="J5" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1715,27 +1727,27 @@
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="14">
         <v>0.54600000000000004</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="16" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="13" t="str">
+      <c r="I6" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="J6" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1748,27 +1760,27 @@
       <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="19">
         <v>3.63</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="16" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="13" t="str">
+      <c r="I7" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="J7" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1779,28 +1791,28 @@
         <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="15">
         <f>CL_/V1_</f>
         <v>6.0975609756097567E-2</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="16" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="13" t="str">
+      <c r="I8" s="11" t="str">
         <f t="shared" ref="I8:I17" ca="1" si="2">_xlfn.IFNA(_xlfn.FORMULATEXT(F8),"")</f>
         <v>=CL_/V1_</v>
       </c>
-      <c r="J8" s="24"/>
-    </row>
-    <row r="9" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1816,23 +1828,23 @@
       <c r="E9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="15">
         <f>Q_/V1_</f>
         <v>0.16646341463414635</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="16" t="s">
         <v>4</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="13" t="str">
+      <c r="I9" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>=Q_/V1_</v>
       </c>
-      <c r="J9" s="24"/>
-    </row>
-    <row r="10" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1848,23 +1860,23 @@
       <c r="E10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="15">
         <f>Q_/V2_</f>
         <v>0.15041322314049588</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="16" t="s">
         <v>4</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="13" t="str">
+      <c r="I10" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>=Q_/V2_</v>
       </c>
-      <c r="J10" s="24"/>
-    </row>
-    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1875,29 +1887,27 @@
         <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="26">
+        <v>74</v>
+      </c>
+      <c r="F11" s="19">
         <v>0</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="16" t="s">
         <v>43</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="13" t="str">
+        <v>72</v>
+      </c>
+      <c r="I11" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J11" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1908,29 +1918,27 @@
         <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="26">
+        <v>75</v>
+      </c>
+      <c r="F12" s="19">
         <v>1</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="16" t="s">
         <v>44</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="13" t="str">
+        <v>72</v>
+      </c>
+      <c r="I12" s="11" t="str">
         <f t="shared" ca="1" si="2"/>
         <v/>
       </c>
-      <c r="J12" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1941,28 +1949,27 @@
         <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="27">
-        <f>Vm*1000/MWD</f>
+      <c r="F13" s="20">
         <v>0</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="16" t="s">
         <v>7</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="13" t="str">
+        <v>72</v>
+      </c>
+      <c r="I13" s="11" t="str">
         <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F13),"")</f>
-        <v>=Vm*1000/MWD</v>
+        <v/>
       </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1973,27 +1980,27 @@
         <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="20">
         <v>1</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="16" t="s">
         <v>15</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="13" t="str">
-        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F14),"")</f>
+        <v>96</v>
+      </c>
+      <c r="I14" s="11" t="str">
+        <f t="shared" ref="I14:I24" ca="1" si="3">_xlfn.IFNA(_xlfn.FORMULATEXT(F14),"")</f>
         <v/>
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2009,57 +2016,57 @@
       <c r="E15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="19">
         <v>145</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="16" t="s">
         <v>30</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+      <c r="I15" s="11" t="str">
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="J15" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="28" t="s">
-        <v>81</v>
+      <c r="C16" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="26">
+        <v>57</v>
+      </c>
+      <c r="F16" s="19">
         <v>33</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="16" t="s">
         <v>30</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+      <c r="I16" s="11" t="str">
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="J16" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2067,632 +2074,672 @@
         <v>36</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="26">
+        <v>58</v>
+      </c>
+      <c r="F17" s="19">
         <v>32</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="16" t="s">
         <v>30</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="13" t="str">
-        <f t="shared" ca="1" si="2"/>
+      <c r="I17" s="11" t="str">
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="J17" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="20">
+        <f>T0*(kon_TL*L0+keT)-koff_TL*TL0</f>
+        <v>0.85749999999999993</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="27">
-        <v>0.45</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I18" s="30" t="s">
-        <v>87</v>
+      <c r="I18" s="11" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=T0*(kon_TL*L0+keT)-koff_TL*TL0</v>
       </c>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>83</v>
+        <v>56</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="26">
-        <v>3</v>
-      </c>
-      <c r="G19" s="23" t="s">
+      <c r="F19" s="19">
+        <v>6</v>
+      </c>
+      <c r="G19" s="16" t="s">
         <v>4</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="I19" s="11" t="str">
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J19" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>83</v>
+        <v>56</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="22">
+        <v>60</v>
+      </c>
+      <c r="F20" s="15">
         <v>6</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="16" t="s">
         <v>4</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="13" t="str">
-        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F20),"")</f>
+      <c r="I20" s="11" t="str">
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="J20" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>83</v>
+        <v>93</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="21">
-        <v>7.47</v>
-      </c>
-      <c r="G21" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="G21" s="16" t="s">
         <v>15</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="13" t="str">
-        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F21),"")</f>
+        <v>17</v>
+      </c>
+      <c r="I21" s="11" t="str">
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="J21" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>24</v>
-      </c>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>83</v>
+        <v>93</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="G22" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="G22" s="16" t="s">
         <v>15</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I22" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="I22" s="11" t="str">
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="J22" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>24.5</v>
-      </c>
+      <c r="J22" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>83</v>
+        <v>91</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F23" s="2">
-        <f>(koff_DT+keDT)/kon_DTn</f>
-        <v>1.2</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>15</v>
+      <c r="F23" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="13" t="str">
-        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F23),"")</f>
-        <v>=(koff_DT+keDT)/kon_DTn</v>
-      </c>
-      <c r="J23" s="7"/>
-    </row>
-    <row r="24" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="I23" s="11" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v/>
+      </c>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="28" t="s">
-        <v>83</v>
+      <c r="C24" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" s="15">
-        <v>3</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>4</v>
+        <v>49</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="13" t="str">
-        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F24),"")</f>
+        <v>17</v>
+      </c>
+      <c r="I24" s="11" t="str">
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="J24" s="8"/>
-    </row>
-    <row r="25" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J24" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>26</v>
+        <v>24.5</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="28" t="s">
-        <v>83</v>
+      <c r="C25" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="17">
-        <f>koff_DT/Kd_DT</f>
-        <v>7.5</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>8</v>
+        <v>85</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="2">
+        <f>Kd_DT+keDT/kon_DT</f>
+        <v>1.6</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="13" t="str">
+      <c r="I25" s="11" t="str">
         <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F25),"")</f>
-        <v>=koff_DT/Kd_DT</v>
-      </c>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+        <v>=Kd_DT+keDT/kon_DT</v>
+      </c>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>27</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>57</v>
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="16">
-        <v>0.03</v>
+        <v>50</v>
+      </c>
+      <c r="F26" s="12">
+        <f>Kd_DT*kon_DT</f>
+        <v>2</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="13"/>
+      <c r="I26" s="11" t="str">
+        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F26),"")</f>
+        <v>=Kd_DT*kon_DT</v>
+      </c>
       <c r="J26" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>28</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>57</v>
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="15">
-        <v>3</v>
+        <v>53</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="24">
+        <v>5</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="13" t="str">
-        <f t="shared" ref="I27:I33" ca="1" si="3">_xlfn.IFNA(_xlfn.FORMULATEXT(F27),"")</f>
+      <c r="I27" s="11" t="str">
+        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F27),"")</f>
         <v/>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J27" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="25">
+        <f>L0*(kon_TL*T0+keL)-koff_TL*TL0</f>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I28" s="11"/>
+      <c r="J28" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="12">
+        <v>6</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="11" t="str">
+        <f t="shared" ref="I29:I34" ca="1" si="4">_xlfn.IFNA(_xlfn.FORMULATEXT(F29),"")</f>
+        <v/>
+      </c>
+      <c r="J29" s="26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="21">
-        <f>1/30</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="G28" s="8" t="s">
+      <c r="B30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="14">
+        <v>6</v>
+      </c>
+      <c r="G30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>30</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" s="15">
-        <v>9.9000000000000008E-3</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
-        <v>31</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="15">
-        <v>10</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="13" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
-      </c>
-      <c r="J30" s="7"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="26" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
-        <v>31.5</v>
-      </c>
-      <c r="B31" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F31" s="15">
-        <f>(koff_TL+F28)/F33</f>
-        <v>10.066666666666666</v>
+        <v>65</v>
+      </c>
+      <c r="F31" s="12">
+        <v>1</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I31" s="13" t="str">
-        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F31),"")</f>
-        <v>=(koff_TL+F28)/F33</v>
+        <v>18</v>
+      </c>
+      <c r="I31" s="11" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
       </c>
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
-        <v>32</v>
-      </c>
-      <c r="B32" s="11" t="s">
+        <v>31.5</v>
+      </c>
+      <c r="B32" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>55</v>
+        <v>81</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="18">
-        <v>5</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="19" t="str">
+        <v>86</v>
+      </c>
+      <c r="F32" s="12">
+        <f>Kd_TL+keTL/kon_TL</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I32" s="11" t="str">
         <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F32),"")</f>
-        <v/>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>52</v>
-      </c>
+        <v>=Kd_TL+keTL/kon_TL</v>
+      </c>
+      <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
-        <v>33</v>
-      </c>
-      <c r="B33" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D33" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>54</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="15">
-        <f>koff_TL/Kd_TL</f>
-        <v>0.5</v>
+        <v>66</v>
+      </c>
+      <c r="F33" s="12">
+        <f>Kd_TL*kon_TL</f>
+        <v>5</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="13" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>=koff_TL/Kd_TL</v>
-      </c>
-      <c r="J33" s="14"/>
+      <c r="I33" s="11" t="str">
+        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F33),"")</f>
+        <v>=Kd_TL*kon_TL</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="12">
+        <v>5</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" s="11" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="F215">
-    <cfRule type="containsText" dxfId="34" priority="54" operator="containsText" text="derived">
-      <formula>NOT(ISERROR(SEARCH("derived",F215)))</formula>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="F216">
+    <cfRule type="containsText" dxfId="22" priority="54" operator="containsText" text="derived">
+      <formula>NOT(ISERROR(SEARCH("derived",F216)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:K1 A34:K1048576 E13:K14 B8:K12 G21:K21 B21:E23 K22:K23 B4:I7 K2:K7 G22:I23 B24:K33 A4:A33 B15:K20">
-    <cfRule type="containsText" dxfId="33" priority="51" operator="containsText" text="calc">
+  <conditionalFormatting sqref="A1:K1 A35:K1048576 E13:K14 B8:K12 B21:E25 K24:K25 B4:I7 K2:K7 G24:I25 B15:K20 G21:K23 A4:A34 B26:K26 I14:I24 B31:K34 B27:I27 B28:E28 G28:I28 B29:I30 K27:K30">
+    <cfRule type="containsText" dxfId="21" priority="51" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1 H4:I1048576">
-    <cfRule type="containsText" dxfId="32" priority="49" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="20" priority="49" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="50" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="19" priority="50" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1 H4:I1048576">
-    <cfRule type="containsText" dxfId="30" priority="44" operator="containsText" text="not used">
+    <cfRule type="containsText" dxfId="18" priority="44" operator="containsText" text="not used">
       <formula>NOT(ISERROR(SEARCH("not used",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="45" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="17" priority="45" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="46" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="16" priority="46" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="47" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="15" priority="47" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="48" operator="containsText" text="check">
+    <cfRule type="containsText" dxfId="14" priority="48" operator="containsText" text="check">
       <formula>NOT(ISERROR(SEARCH("check",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1 H4:H1048576">
-    <cfRule type="containsText" dxfId="25" priority="43" operator="containsText" text="internal data">
+    <cfRule type="containsText" dxfId="13" priority="43" operator="containsText" text="internal data">
       <formula>NOT(ISERROR(SEARCH("internal data",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:I3">
-    <cfRule type="containsText" dxfId="24" priority="15" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:I3">
-    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:I3">
-    <cfRule type="containsText" dxfId="21" priority="8" operator="containsText" text="not used">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="not used">
       <formula>NOT(ISERROR(SEARCH("not used",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="10" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="11" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="12" operator="containsText" text="check">
+    <cfRule type="containsText" dxfId="5" priority="12" operator="containsText" text="check">
       <formula>NOT(ISERROR(SEARCH("check",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H3">
-    <cfRule type="containsText" dxfId="16" priority="7" operator="containsText" text="internal data">
+    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="internal data">
       <formula>NOT(ISERROR(SEARCH("internal data",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:D14">
-    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F23">
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="calc">
-      <formula>NOT(ISERROR(SEARCH("calc",F22)))</formula>
+  <conditionalFormatting sqref="F24:F25">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="calc">
+      <formula>NOT(ISERROR(SEARCH("calc",F24)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J22:J23">
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="calc">
-      <formula>NOT(ISERROR(SEARCH("calc",J22)))</formula>
+  <conditionalFormatting sqref="J24:J25">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="calc">
+      <formula>NOT(ISERROR(SEARCH("calc",J24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",J2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>